<commit_message>
Fix ESLint warnings and improve data processing
</commit_message>
<xml_diff>
--- a/public/sales_data.xlsx
+++ b/public/sales_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shavinsergey/sales-dashboard/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3576280F-61A3-3D45-A209-ECFBE9AAE03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D10554-8A4F-3745-9FE1-97B3A1935B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="3840" windowWidth="21840" windowHeight="13140" xr2:uid="{CFD313C6-8799-4299-A8F9-C915DE26A65D}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="29">
   <si>
     <t>Week</t>
   </si>
@@ -113,12 +113,15 @@
   <si>
     <t>CTR</t>
   </si>
+  <si>
+    <t>Группа 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +269,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="204"/>
@@ -991,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE2CC5B-4398-406D-8FDE-300DFA760354}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N41"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1276,37 +1286,37 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>3086018</v>
+        <v>4262509.4000000004</v>
       </c>
       <c r="E7">
-        <v>3016018</v>
+        <v>4192509</v>
       </c>
       <c r="F7">
-        <v>16.8</v>
+        <v>17.14</v>
       </c>
       <c r="G7">
-        <v>1.2</v>
+        <v>4.84</v>
       </c>
       <c r="H7">
-        <v>137672</v>
+        <v>214831.2</v>
       </c>
       <c r="I7">
-        <v>2854715</v>
+        <v>4164751.3</v>
       </c>
       <c r="J7" t="s">
         <v>20</v>
       </c>
       <c r="K7">
-        <v>12</v>
+        <v>171.2</v>
       </c>
       <c r="L7" s="1">
         <v>0.1</v>
@@ -1323,43 +1333,43 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>3086018</v>
+      </c>
+      <c r="E8">
+        <v>3016018</v>
+      </c>
+      <c r="F8">
+        <v>16.8</v>
+      </c>
+      <c r="G8">
+        <v>1.2</v>
+      </c>
+      <c r="H8">
+        <v>137672</v>
+      </c>
+      <c r="I8">
+        <v>2854715</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8">
         <v>12</v>
       </c>
-      <c r="D8">
-        <v>3654507</v>
-      </c>
-      <c r="E8">
-        <v>3554507</v>
-      </c>
-      <c r="F8">
-        <v>15.1</v>
-      </c>
-      <c r="G8">
-        <v>2.8</v>
-      </c>
-      <c r="H8">
-        <v>152021</v>
-      </c>
-      <c r="I8">
-        <v>3252029</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
       <c r="L8" s="1">
-        <v>0.115</v>
+        <v>0.1</v>
       </c>
       <c r="M8" s="1">
-        <v>0.14199999999999999</v>
+        <v>0.121</v>
       </c>
       <c r="N8" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1367,43 +1377,43 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9">
-        <v>2681867</v>
+        <v>3654507</v>
       </c>
       <c r="E9">
-        <v>2581867</v>
+        <v>3554507</v>
       </c>
       <c r="F9">
-        <v>18.7</v>
+        <v>15.1</v>
       </c>
       <c r="G9">
-        <v>4.0999999999999996</v>
+        <v>2.8</v>
       </c>
       <c r="H9">
-        <v>165687</v>
+        <v>152021</v>
       </c>
       <c r="I9">
-        <v>2589201</v>
+        <v>3252029</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K9">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="L9" s="1">
-        <v>0.13</v>
+        <v>0.115</v>
       </c>
       <c r="M9" s="1">
-        <v>0.16300000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="N9" s="1">
-        <v>4.7E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1411,43 +1421,43 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>4385623</v>
+        <v>2681867</v>
       </c>
       <c r="E10">
-        <v>4285623</v>
+        <v>2581867</v>
       </c>
       <c r="F10">
-        <v>15.5</v>
+        <v>18.7</v>
       </c>
       <c r="G10">
-        <v>2.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H10">
-        <v>187283</v>
+        <v>165687</v>
       </c>
       <c r="I10">
-        <v>4150000</v>
+        <v>2589201</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K10">
-        <v>56.75</v>
+        <v>78</v>
       </c>
       <c r="L10" s="1">
-        <v>0.14499999999999999</v>
+        <v>0.13</v>
       </c>
       <c r="M10" s="1">
-        <v>0.184</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="N10" s="1">
-        <v>5.1999999999999998E-2</v>
+        <v>4.7E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1455,131 +1465,131 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11">
-        <v>4056478</v>
+        <v>4385623</v>
       </c>
       <c r="E11">
-        <v>3956478</v>
+        <v>4285623</v>
       </c>
       <c r="F11">
-        <v>17.8</v>
+        <v>15.5</v>
       </c>
       <c r="G11">
-        <v>4.4000000000000004</v>
+        <v>2.9</v>
       </c>
       <c r="H11">
-        <v>201654</v>
+        <v>187283</v>
       </c>
       <c r="I11">
-        <v>3850000</v>
+        <v>4150000</v>
       </c>
       <c r="J11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K11">
-        <v>54.3333333333333</v>
+        <v>56.75</v>
       </c>
       <c r="L11" s="1">
-        <v>0.16</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="M11" s="1">
-        <v>0.20499999999999999</v>
+        <v>0.184</v>
       </c>
       <c r="N11" s="1">
-        <v>5.7000000000000002E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D12">
-        <v>3156018</v>
+        <v>4056478</v>
       </c>
       <c r="E12">
-        <v>3086018</v>
+        <v>3956478</v>
       </c>
       <c r="F12">
-        <v>17</v>
+        <v>17.8</v>
       </c>
       <c r="G12">
-        <v>1.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H12">
-        <v>140672</v>
+        <v>201654</v>
       </c>
       <c r="I12">
-        <v>2924715</v>
+        <v>3850000</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K12">
-        <v>51.9166666666666</v>
+        <v>54.3333333333333</v>
       </c>
       <c r="L12" s="1">
-        <v>0.17499999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="M12" s="1">
-        <v>0.22600000000000001</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="N12" s="1">
-        <v>6.2E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>3754507</v>
+        <v>4374509.4000000004</v>
       </c>
       <c r="E13">
-        <v>3654507</v>
+        <v>4262509.4000000004</v>
       </c>
       <c r="F13">
-        <v>15.4</v>
+        <v>17.5</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>5.03</v>
       </c>
       <c r="H13">
-        <v>155021</v>
+        <v>217831.2</v>
       </c>
       <c r="I13">
-        <v>3312029</v>
+        <v>4205751.3</v>
       </c>
       <c r="J13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K13">
-        <v>49.5</v>
+        <v>82.341666666666598</v>
       </c>
       <c r="L13" s="1">
-        <v>0.19</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="M13" s="1">
-        <v>0.247</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="N13" s="1">
-        <v>6.7000000000000004E-2</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1587,43 +1597,43 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>2781867</v>
+        <v>3156018</v>
       </c>
       <c r="E14">
-        <v>2681867</v>
+        <v>3086018</v>
       </c>
       <c r="F14">
-        <v>19.100000000000001</v>
+        <v>17</v>
       </c>
       <c r="G14">
-        <v>4.3</v>
+        <v>1.3</v>
       </c>
       <c r="H14">
-        <v>168687</v>
+        <v>140672</v>
       </c>
       <c r="I14">
-        <v>2639201</v>
+        <v>2924715</v>
       </c>
       <c r="J14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K14">
-        <v>47.0833333333333</v>
+        <v>51.9166666666666</v>
       </c>
       <c r="L14" s="1">
-        <v>0.20499999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="M14" s="1">
-        <v>0.26800000000000002</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="N14" s="1">
-        <v>7.1999999999999995E-2</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -1631,43 +1641,43 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D15">
-        <v>4485623</v>
+        <v>3754507</v>
       </c>
       <c r="E15">
-        <v>4385623</v>
+        <v>3654507</v>
       </c>
       <c r="F15">
-        <v>15.8</v>
+        <v>15.4</v>
       </c>
       <c r="G15">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="H15">
-        <v>190283</v>
+        <v>155021</v>
       </c>
       <c r="I15">
-        <v>4200000</v>
+        <v>3312029</v>
       </c>
       <c r="J15" t="s">
         <v>22</v>
       </c>
       <c r="K15">
-        <v>44.6666666666666</v>
+        <v>49.5</v>
       </c>
       <c r="L15" s="1">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="M15" s="1">
-        <v>0.28899999999999998</v>
+        <v>0.247</v>
       </c>
       <c r="N15" s="1">
-        <v>7.6999999999999999E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -1675,175 +1685,175 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D16">
-        <v>4156478</v>
+        <v>2781867</v>
       </c>
       <c r="E16">
-        <v>4056478</v>
+        <v>2681867</v>
       </c>
       <c r="F16">
-        <v>18.100000000000001</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="G16">
-        <v>4.5999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="H16">
-        <v>204654</v>
+        <v>168687</v>
       </c>
       <c r="I16">
-        <v>3900000</v>
+        <v>2639201</v>
       </c>
       <c r="J16" t="s">
         <v>23</v>
       </c>
       <c r="K16">
-        <v>42.25</v>
+        <v>47.0833333333333</v>
       </c>
       <c r="L16" s="1">
-        <v>0.23499999999999999</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="M16" s="1">
-        <v>0.31</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="N16" s="1">
-        <v>8.2000000000000003E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D17">
-        <v>3226018</v>
+        <v>4485623</v>
       </c>
       <c r="E17">
-        <v>3156018</v>
+        <v>4385623</v>
       </c>
       <c r="F17">
-        <v>17.2</v>
+        <v>15.8</v>
       </c>
       <c r="G17">
-        <v>1.4</v>
+        <v>3.1</v>
       </c>
       <c r="H17">
-        <v>143672</v>
+        <v>190283</v>
       </c>
       <c r="I17">
-        <v>2994715</v>
+        <v>4200000</v>
       </c>
       <c r="J17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K17">
-        <v>39.8333333333333</v>
+        <v>44.6666666666666</v>
       </c>
       <c r="L17" s="1">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="M17" s="1">
-        <v>0.33100000000000002</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="N17" s="1">
-        <v>8.6999999999999994E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D18">
-        <v>3854507</v>
+        <v>4156478</v>
       </c>
       <c r="E18">
-        <v>3754507</v>
+        <v>4056478</v>
       </c>
       <c r="F18">
-        <v>15.7</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="G18">
-        <v>3.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H18">
-        <v>158021</v>
+        <v>204654</v>
       </c>
       <c r="I18">
-        <v>3372029</v>
+        <v>3900000</v>
       </c>
       <c r="J18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K18">
-        <v>37.4166666666666</v>
+        <v>42.25</v>
       </c>
       <c r="L18" s="1">
-        <v>0.26500000000000001</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="M18" s="1">
-        <v>0.35199999999999998</v>
+        <v>0.31</v>
       </c>
       <c r="N18" s="1">
-        <v>9.1999999999999998E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>2881867</v>
+        <v>4486509.4000000004</v>
       </c>
       <c r="E19">
-        <v>2781867</v>
+        <v>4374509.4000000004</v>
       </c>
       <c r="F19">
-        <v>19.5</v>
+        <v>17.86</v>
       </c>
       <c r="G19">
-        <v>4.5</v>
+        <v>5.27</v>
       </c>
       <c r="H19">
-        <v>171687</v>
+        <v>220831.2</v>
       </c>
       <c r="I19">
-        <v>2689201</v>
+        <v>4246751.3</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K19">
-        <v>35</v>
+        <v>39.833333333333599</v>
       </c>
       <c r="L19" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="M19" s="1">
-        <v>0.373</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="N19" s="1">
-        <v>9.7000000000000003E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -1851,43 +1861,43 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D20">
-        <v>4585623</v>
+        <v>3226018</v>
       </c>
       <c r="E20">
-        <v>4485623</v>
+        <v>3156018</v>
       </c>
       <c r="F20">
-        <v>16.100000000000001</v>
+        <v>17.2</v>
       </c>
       <c r="G20">
-        <v>3.3</v>
+        <v>1.4</v>
       </c>
       <c r="H20">
-        <v>193283</v>
+        <v>143672</v>
       </c>
       <c r="I20">
-        <v>4250000</v>
+        <v>2994715</v>
       </c>
       <c r="J20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K20">
-        <v>32.5833333333333</v>
+        <v>39.8333333333333</v>
       </c>
       <c r="L20" s="1">
-        <v>0.29499999999999998</v>
+        <v>0.25</v>
       </c>
       <c r="M20" s="1">
-        <v>0.39400000000000002</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="N20" s="1">
-        <v>0.10199999999999999</v>
+        <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -1895,219 +1905,219 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D21">
-        <v>4256478</v>
+        <v>3854507</v>
       </c>
       <c r="E21">
-        <v>4156478</v>
+        <v>3754507</v>
       </c>
       <c r="F21">
-        <v>18.399999999999999</v>
+        <v>15.7</v>
       </c>
       <c r="G21">
-        <v>4.8</v>
+        <v>3.2</v>
       </c>
       <c r="H21">
-        <v>207654</v>
+        <v>158021</v>
       </c>
       <c r="I21">
-        <v>3950000</v>
+        <v>3372029</v>
       </c>
       <c r="J21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K21">
-        <v>30.1666666666666</v>
+        <v>37.4166666666666</v>
       </c>
       <c r="L21" s="1">
-        <v>0.31</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="M21" s="1">
-        <v>0.41499999999999998</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="N21" s="1">
-        <v>0.107</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D22">
-        <v>3296018</v>
+        <v>2881867</v>
       </c>
       <c r="E22">
-        <v>3226018</v>
+        <v>2781867</v>
       </c>
       <c r="F22">
-        <v>17.399999999999999</v>
+        <v>19.5</v>
       </c>
       <c r="G22">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="H22">
-        <v>146672</v>
+        <v>171687</v>
       </c>
       <c r="I22">
-        <v>3064715</v>
+        <v>2689201</v>
       </c>
       <c r="J22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K22">
-        <v>27.75</v>
+        <v>35</v>
       </c>
       <c r="L22" s="1">
-        <v>0.32500000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="M22" s="1">
-        <v>0.436</v>
+        <v>0.373</v>
       </c>
       <c r="N22" s="1">
-        <v>0.112</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D23">
-        <v>3954507</v>
+        <v>4585623</v>
       </c>
       <c r="E23">
-        <v>3854507</v>
+        <v>4485623</v>
       </c>
       <c r="F23">
-        <v>16</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G23">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="H23">
-        <v>161021</v>
+        <v>193283</v>
       </c>
       <c r="I23">
-        <v>3432029</v>
+        <v>4250000</v>
       </c>
       <c r="J23" t="s">
         <v>22</v>
       </c>
       <c r="K23">
-        <v>25.3333333333333</v>
+        <v>32.5833333333333</v>
       </c>
       <c r="L23" s="1">
-        <v>0.34</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="M23" s="1">
-        <v>0.45700000000000002</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="N23" s="1">
-        <v>0.11700000000000001</v>
+        <v>0.10199999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D24">
-        <v>2981867</v>
+        <v>4256478</v>
       </c>
       <c r="E24">
-        <v>2881867</v>
+        <v>4156478</v>
       </c>
       <c r="F24">
-        <v>19.899999999999999</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="G24">
-        <v>4.7</v>
+        <v>4.8</v>
       </c>
       <c r="H24">
-        <v>174687</v>
+        <v>207654</v>
       </c>
       <c r="I24">
-        <v>2739201</v>
+        <v>3950000</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
       <c r="K24">
-        <v>22.9166666666666</v>
+        <v>30.1666666666666</v>
       </c>
       <c r="L24" s="1">
-        <v>0.35499999999999998</v>
+        <v>0.31</v>
       </c>
       <c r="M24" s="1">
-        <v>0.47799999999999998</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="N24" s="1">
-        <v>0.122</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>4685623</v>
+        <v>4598509.4000000004</v>
       </c>
       <c r="E25">
-        <v>4585623</v>
+        <v>4486509.4000000004</v>
       </c>
       <c r="F25">
-        <v>16.399999999999999</v>
+        <v>18.22</v>
       </c>
       <c r="G25">
-        <v>3.5</v>
+        <v>5.51</v>
       </c>
       <c r="H25">
-        <v>196283</v>
+        <v>223831.2</v>
       </c>
       <c r="I25">
-        <v>4300000</v>
+        <v>4287751.3</v>
       </c>
       <c r="J25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K25">
-        <v>20.5</v>
+        <v>27.749999999999801</v>
       </c>
       <c r="L25" s="1">
-        <v>0.37</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="M25" s="1">
-        <v>0.499</v>
+        <v>0.436</v>
       </c>
       <c r="N25" s="1">
-        <v>0.127</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -2115,268 +2125,268 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D26">
-        <v>4356478</v>
+        <v>3296018</v>
       </c>
       <c r="E26">
-        <v>4256478</v>
+        <v>3226018</v>
       </c>
       <c r="F26">
-        <v>18.7</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="H26">
-        <v>210654</v>
+        <v>146672</v>
       </c>
       <c r="I26">
-        <v>4000000</v>
+        <v>3064715</v>
       </c>
       <c r="J26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K26">
-        <v>18.0833333333333</v>
+        <v>27.75</v>
       </c>
       <c r="L26" s="1">
-        <v>0.38500000000000001</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="M26" s="1">
-        <v>0.52</v>
+        <v>0.436</v>
       </c>
       <c r="N26" s="1">
-        <v>0.13200000000000001</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D27">
-        <v>3366018</v>
+        <v>3954507</v>
       </c>
       <c r="E27">
-        <v>3296018</v>
+        <v>3854507</v>
       </c>
       <c r="F27">
-        <v>17.600000000000001</v>
+        <v>16</v>
       </c>
       <c r="G27">
-        <v>1.6</v>
+        <v>3.4</v>
       </c>
       <c r="H27">
-        <v>149672</v>
+        <v>161021</v>
       </c>
       <c r="I27">
-        <v>3134715</v>
+        <v>3432029</v>
       </c>
       <c r="J27" t="s">
         <v>22</v>
       </c>
       <c r="K27">
-        <v>15.6666666666666</v>
+        <v>25.3333333333333</v>
       </c>
       <c r="L27" s="1">
-        <v>0.4</v>
+        <v>0.34</v>
       </c>
       <c r="M27" s="1">
-        <v>0.54100000000000004</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="N27" s="1">
-        <v>0.13700000000000001</v>
+        <v>0.11700000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>4054507</v>
+        <v>2981867</v>
       </c>
       <c r="E28">
-        <v>3954507</v>
+        <v>2881867</v>
       </c>
       <c r="F28">
-        <v>16.3</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G28">
-        <v>3.6</v>
+        <v>4.7</v>
       </c>
       <c r="H28">
-        <v>164021</v>
+        <v>174687</v>
       </c>
       <c r="I28">
-        <v>3492029</v>
+        <v>2739201</v>
       </c>
       <c r="J28" t="s">
         <v>23</v>
       </c>
       <c r="K28">
-        <v>13.25</v>
+        <v>22.9166666666666</v>
       </c>
       <c r="L28" s="1">
-        <v>0.41499999999999998</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="M28" s="1">
-        <v>0.56200000000000006</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="N28" s="1">
-        <v>0.14199999999999999</v>
+        <v>0.122</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29">
-        <v>3081867</v>
+        <v>4685623</v>
       </c>
       <c r="E29">
-        <v>2981867</v>
+        <v>4585623</v>
       </c>
       <c r="F29">
-        <v>20.3</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="G29">
-        <v>4.9000000000000004</v>
+        <v>3.5</v>
       </c>
       <c r="H29">
-        <v>177687</v>
+        <v>196283</v>
       </c>
       <c r="I29">
-        <v>2789201</v>
+        <v>4300000</v>
       </c>
       <c r="J29" t="s">
         <v>22</v>
       </c>
       <c r="K29">
-        <v>10.8333333333333</v>
+        <v>20.5</v>
       </c>
       <c r="L29" s="1">
-        <v>0.43</v>
+        <v>0.37</v>
       </c>
       <c r="M29" s="1">
-        <v>0.58299999999999996</v>
+        <v>0.499</v>
       </c>
       <c r="N29" s="1">
-        <v>0.14699999999999999</v>
+        <v>0.127</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D30">
-        <v>4785623</v>
+        <v>4356478</v>
       </c>
       <c r="E30">
-        <v>4685623</v>
+        <v>4256478</v>
       </c>
       <c r="F30">
-        <v>16.7</v>
+        <v>18.7</v>
       </c>
       <c r="G30">
-        <v>3.7</v>
+        <v>5</v>
       </c>
       <c r="H30">
-        <v>199283</v>
+        <v>210654</v>
       </c>
       <c r="I30">
-        <v>4350000</v>
+        <v>4000000</v>
       </c>
       <c r="J30" t="s">
         <v>23</v>
       </c>
       <c r="K30">
-        <v>8.4166666666666305</v>
+        <v>18.0833333333333</v>
       </c>
       <c r="L30" s="1">
-        <v>0.44500000000000001</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="M30" s="1">
-        <v>0.60399999999999998</v>
+        <v>0.52</v>
       </c>
       <c r="N30" s="1">
-        <v>0.152</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D31">
-        <v>4456478</v>
+        <v>4710509.4000000004</v>
       </c>
       <c r="E31">
-        <v>4356478</v>
+        <v>4598509.4000000004</v>
       </c>
       <c r="F31">
-        <v>19</v>
+        <v>18.579999999999998</v>
       </c>
       <c r="G31">
-        <v>5.2</v>
+        <v>5.75</v>
       </c>
       <c r="H31">
-        <v>213654</v>
+        <v>226831.2</v>
       </c>
       <c r="I31">
-        <v>4050000</v>
+        <v>4328751.3</v>
       </c>
       <c r="J31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K31">
-        <v>6.0000000000000302</v>
+        <v>15.666666666666501</v>
       </c>
       <c r="L31" s="1">
-        <v>0.46</v>
+        <v>0.4</v>
       </c>
       <c r="M31" s="1">
-        <v>0.625</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="N31" s="1">
-        <v>0.157</v>
+        <v>0.13700000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
@@ -2385,42 +2395,42 @@
         <v>10</v>
       </c>
       <c r="D32">
-        <v>3436018</v>
+        <v>3366018</v>
       </c>
       <c r="E32">
-        <v>3366018</v>
+        <v>3296018</v>
       </c>
       <c r="F32">
-        <v>17.8</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="G32">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="H32">
-        <v>152672</v>
+        <v>149672</v>
       </c>
       <c r="I32">
-        <v>3204715</v>
+        <v>3134715</v>
       </c>
       <c r="J32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K32">
-        <v>3.5833333333333299</v>
+        <v>15.6666666666666</v>
       </c>
       <c r="L32" s="1">
-        <v>0.47499999999999998</v>
+        <v>0.4</v>
       </c>
       <c r="M32" s="1">
-        <v>0.64600000000000002</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="N32" s="1">
-        <v>0.16200000000000001</v>
+        <v>0.13700000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -2429,42 +2439,42 @@
         <v>12</v>
       </c>
       <c r="D33">
-        <v>4154507</v>
+        <v>4054507</v>
       </c>
       <c r="E33">
-        <v>4054507</v>
+        <v>3954507</v>
       </c>
       <c r="F33">
-        <v>16.600000000000001</v>
+        <v>16.3</v>
       </c>
       <c r="G33">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="H33">
-        <v>167021</v>
+        <v>164021</v>
       </c>
       <c r="I33">
-        <v>3552029</v>
+        <v>3492029</v>
       </c>
       <c r="J33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K33">
-        <v>1.1666666666666301</v>
+        <v>13.25</v>
       </c>
       <c r="L33" s="1">
-        <v>0.49</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="M33" s="1">
-        <v>0.66700000000000004</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="N33" s="1">
-        <v>0.16700000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
@@ -2473,42 +2483,42 @@
         <v>14</v>
       </c>
       <c r="D34">
-        <v>3181867</v>
+        <v>3081867</v>
       </c>
       <c r="E34">
-        <v>3081867</v>
+        <v>2981867</v>
       </c>
       <c r="F34">
-        <v>20.7</v>
+        <v>20.3</v>
       </c>
       <c r="G34">
-        <v>5.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H34">
-        <v>180687</v>
+        <v>177687</v>
       </c>
       <c r="I34">
-        <v>2839201</v>
+        <v>2789201</v>
       </c>
       <c r="J34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K34">
-        <v>-1.24999999999997</v>
+        <v>10.8333333333333</v>
       </c>
       <c r="L34" s="1">
-        <v>0.505</v>
+        <v>0.43</v>
       </c>
       <c r="M34" s="1">
-        <v>0.68799999999999994</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="N34" s="1">
-        <v>0.17199999999999999</v>
+        <v>0.14699999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
@@ -2517,42 +2527,42 @@
         <v>16</v>
       </c>
       <c r="D35">
-        <v>4885623</v>
+        <v>4785623</v>
       </c>
       <c r="E35">
-        <v>4785623</v>
+        <v>4685623</v>
       </c>
       <c r="F35">
-        <v>17</v>
+        <v>16.7</v>
       </c>
       <c r="G35">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="H35">
-        <v>202283</v>
+        <v>199283</v>
       </c>
       <c r="I35">
-        <v>4400000</v>
+        <v>4350000</v>
       </c>
       <c r="J35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K35">
-        <v>-3.6666666666666701</v>
+        <v>8.4166666666666305</v>
       </c>
       <c r="L35" s="1">
-        <v>0.52</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="M35" s="1">
-        <v>0.70899999999999996</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="N35" s="1">
-        <v>0.17699999999999999</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
@@ -2561,260 +2571,613 @@
         <v>18</v>
       </c>
       <c r="D36">
-        <v>4556478</v>
+        <v>4456478</v>
       </c>
       <c r="E36">
-        <v>4456478</v>
+        <v>4356478</v>
       </c>
       <c r="F36">
-        <v>19.3</v>
+        <v>19</v>
       </c>
       <c r="G36">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
       <c r="H36">
-        <v>216654</v>
+        <v>213654</v>
       </c>
       <c r="I36">
-        <v>4100000</v>
+        <v>4050000</v>
       </c>
       <c r="J36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K36">
-        <v>-6.0833333333333703</v>
+        <v>6.0000000000000302</v>
       </c>
       <c r="L36" s="1">
-        <v>0.53500000000000003</v>
+        <v>0.46</v>
       </c>
       <c r="M36" s="1">
-        <v>0.73</v>
+        <v>0.625</v>
       </c>
       <c r="N36" s="1">
-        <v>0.182</v>
+        <v>0.157</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
       </c>
       <c r="D37">
-        <v>3506018</v>
+        <v>4822509.4000000004</v>
       </c>
       <c r="E37">
-        <v>3436018</v>
+        <v>4710509.4000000004</v>
       </c>
       <c r="F37">
-        <v>18</v>
+        <v>18.940000000000001</v>
       </c>
       <c r="G37">
-        <v>1.8</v>
+        <v>5.99</v>
       </c>
       <c r="H37">
-        <v>155672</v>
+        <v>229831.2</v>
       </c>
       <c r="I37">
-        <v>3274715</v>
+        <v>4369751.3</v>
       </c>
       <c r="J37" t="s">
         <v>22</v>
       </c>
       <c r="K37">
-        <v>-8.4999999999999698</v>
+        <v>3.5833333333335999</v>
       </c>
       <c r="L37" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="M37" s="1">
-        <v>0.751</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="N37" s="1">
-        <v>0.187</v>
+        <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D38">
-        <v>4254507</v>
+        <v>3436018</v>
       </c>
       <c r="E38">
-        <v>4154507</v>
+        <v>3366018</v>
       </c>
       <c r="F38">
-        <v>16.899999999999999</v>
+        <v>17.8</v>
       </c>
       <c r="G38">
-        <v>4</v>
+        <v>1.7</v>
       </c>
       <c r="H38">
-        <v>170021</v>
+        <v>152672</v>
       </c>
       <c r="I38">
-        <v>3612029</v>
+        <v>3204715</v>
       </c>
       <c r="J38" t="s">
         <v>23</v>
       </c>
       <c r="K38">
-        <v>-10.9166666666667</v>
+        <v>3.5833333333333299</v>
       </c>
       <c r="L38" s="1">
-        <v>0.56499999999999995</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="M38" s="1">
-        <v>0.77200000000000002</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="N38" s="1">
-        <v>0.192</v>
+        <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D39">
-        <v>3281867</v>
+        <v>4154507</v>
       </c>
       <c r="E39">
-        <v>3181867</v>
+        <v>4054507</v>
       </c>
       <c r="F39">
-        <v>21.1</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="G39">
-        <v>5.3</v>
+        <v>3.8</v>
       </c>
       <c r="H39">
-        <v>183687</v>
+        <v>167021</v>
       </c>
       <c r="I39">
-        <v>2889201</v>
+        <v>3552029</v>
       </c>
       <c r="J39" t="s">
         <v>22</v>
       </c>
       <c r="K39">
-        <v>-13.3333333333334</v>
+        <v>1.1666666666666301</v>
       </c>
       <c r="L39" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.49</v>
       </c>
       <c r="M39" s="1">
-        <v>0.79300000000000004</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="N39" s="1">
-        <v>0.19700000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D40">
-        <v>4985623</v>
+        <v>3181867</v>
       </c>
       <c r="E40">
-        <v>4885623</v>
+        <v>3081867</v>
       </c>
       <c r="F40">
-        <v>17.3</v>
+        <v>20.7</v>
       </c>
       <c r="G40">
-        <v>4.0999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H40">
-        <v>205283</v>
+        <v>180687</v>
       </c>
       <c r="I40">
-        <v>4450000</v>
+        <v>2839201</v>
       </c>
       <c r="J40" t="s">
         <v>23</v>
       </c>
       <c r="K40">
-        <v>-15.75</v>
+        <v>-1.24999999999997</v>
       </c>
       <c r="L40" s="1">
-        <v>0.59499999999999997</v>
+        <v>0.505</v>
       </c>
       <c r="M40" s="1">
-        <v>0.81399999999999995</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="N40" s="1">
-        <v>0.20200000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <v>4885623</v>
+      </c>
+      <c r="E41">
+        <v>4785623</v>
+      </c>
+      <c r="F41">
         <v>17</v>
       </c>
-      <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41">
-        <v>4656478</v>
-      </c>
-      <c r="E41">
-        <v>4556478</v>
-      </c>
-      <c r="F41">
-        <v>19.600000000000001</v>
-      </c>
       <c r="G41">
-        <v>5.6</v>
+        <v>3.9</v>
       </c>
       <c r="H41">
-        <v>219654</v>
+        <v>202283</v>
       </c>
       <c r="I41">
-        <v>4150000</v>
+        <v>4400000</v>
       </c>
       <c r="J41" t="s">
         <v>22</v>
       </c>
       <c r="K41">
+        <v>-3.6666666666666701</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="N41" s="1">
+        <v>0.17699999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42">
+        <v>4556478</v>
+      </c>
+      <c r="E42">
+        <v>4456478</v>
+      </c>
+      <c r="F42">
+        <v>19.3</v>
+      </c>
+      <c r="G42">
+        <v>5.4</v>
+      </c>
+      <c r="H42">
+        <v>216654</v>
+      </c>
+      <c r="I42">
+        <v>4100000</v>
+      </c>
+      <c r="J42" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42">
+        <v>-6.0833333333333703</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="N42" s="1">
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>4934509.4000000004</v>
+      </c>
+      <c r="E43">
+        <v>4822509.4000000004</v>
+      </c>
+      <c r="F43">
+        <v>19.3</v>
+      </c>
+      <c r="G43">
+        <v>6.23</v>
+      </c>
+      <c r="H43">
+        <v>232831.2</v>
+      </c>
+      <c r="I43">
+        <v>4410751.3</v>
+      </c>
+      <c r="J43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43">
+        <v>-8.5000000000001705</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0.751</v>
+      </c>
+      <c r="N43" s="1">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>3506018</v>
+      </c>
+      <c r="E44">
+        <v>3436018</v>
+      </c>
+      <c r="F44">
+        <v>18</v>
+      </c>
+      <c r="G44">
+        <v>1.8</v>
+      </c>
+      <c r="H44">
+        <v>155672</v>
+      </c>
+      <c r="I44">
+        <v>3274715</v>
+      </c>
+      <c r="J44" t="s">
+        <v>22</v>
+      </c>
+      <c r="K44">
+        <v>-8.4999999999999698</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M44" s="1">
+        <v>0.751</v>
+      </c>
+      <c r="N44" s="1">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45">
+        <v>4254507</v>
+      </c>
+      <c r="E45">
+        <v>4154507</v>
+      </c>
+      <c r="F45">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45">
+        <v>170021</v>
+      </c>
+      <c r="I45">
+        <v>3612029</v>
+      </c>
+      <c r="J45" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45">
+        <v>-10.9166666666667</v>
+      </c>
+      <c r="L45" s="1">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="M45" s="1">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="N45" s="1">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46">
+        <v>3281867</v>
+      </c>
+      <c r="E46">
+        <v>3181867</v>
+      </c>
+      <c r="F46">
+        <v>21.1</v>
+      </c>
+      <c r="G46">
+        <v>5.3</v>
+      </c>
+      <c r="H46">
+        <v>183687</v>
+      </c>
+      <c r="I46">
+        <v>2889201</v>
+      </c>
+      <c r="J46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K46">
+        <v>-13.3333333333334</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="M46" s="1">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="N46" s="1">
+        <v>0.19700000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>4985623</v>
+      </c>
+      <c r="E47">
+        <v>4885623</v>
+      </c>
+      <c r="F47">
+        <v>17.3</v>
+      </c>
+      <c r="G47">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H47">
+        <v>205283</v>
+      </c>
+      <c r="I47">
+        <v>4450000</v>
+      </c>
+      <c r="J47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K47">
+        <v>-15.75</v>
+      </c>
+      <c r="L47" s="1">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="M47" s="1">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="N47" s="1">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48">
+        <v>4656478</v>
+      </c>
+      <c r="E48">
+        <v>4556478</v>
+      </c>
+      <c r="F48">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="G48">
+        <v>5.6</v>
+      </c>
+      <c r="H48">
+        <v>219654</v>
+      </c>
+      <c r="I48">
+        <v>4150000</v>
+      </c>
+      <c r="J48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K48">
         <v>-18.1666666666667</v>
       </c>
-      <c r="L41" s="1">
+      <c r="L48" s="1">
         <v>0.61</v>
       </c>
-      <c r="M41" s="1">
+      <c r="M48" s="1">
         <v>0.83499999999999996</v>
       </c>
-      <c r="N41" s="1">
+      <c r="N48" s="1">
         <v>0.20699999999999999</v>
       </c>
     </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>5046509.4000000004</v>
+      </c>
+      <c r="E49">
+        <v>4934509.4000000004</v>
+      </c>
+      <c r="F49">
+        <v>19.66</v>
+      </c>
+      <c r="G49">
+        <v>6.47</v>
+      </c>
+      <c r="H49">
+        <v>235831.2</v>
+      </c>
+      <c r="I49">
+        <v>4451751.3</v>
+      </c>
+      <c r="J49" t="s">
+        <v>22</v>
+      </c>
+      <c r="K49">
+        <v>-20.583333333333702</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="M49" s="1">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="N49" s="1">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>